<commit_message>
Add optional is_rehydrated field
</commit_message>
<xml_diff>
--- a/sample-section/latest/sample-section.xlsx
+++ b/sample-section/latest/sample-section.xlsx
@@ -15,7 +15,8 @@
     <sheet name="storage_method" r:id="rId9" sheetId="7"/>
     <sheet name="thickness_unit" r:id="rId10" sheetId="8"/>
     <sheet name="area_unit" r:id="rId11" sheetId="9"/>
-    <sheet name=".metadata" r:id="rId12" sheetId="10"/>
+    <sheet name="is_rehydrated" r:id="rId12" sheetId="10"/>
+    <sheet name=".metadata" r:id="rId13" sheetId="11"/>
   </sheets>
 </workbook>
 </file>
@@ -144,11 +145,16 @@
     </comment>
     <comment ref="T1" authorId="1">
       <text>
+        <t>Was the section rehydrated?</t>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="1">
+      <text>
         <t>Miscellaneous details about the sample, not captured in the existing metadata
 fields.</t>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="V1" authorId="1">
       <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
@@ -160,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>source_id</t>
   </si>
@@ -219,30 +225,30 @@
     <t>http://purl.obolibrary.org/obo/OBI_0100046</t>
   </si>
   <si>
-    <t>NBF (Neutral Buffered Formalin)</t>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
+  </si>
+  <si>
+    <t>Allprotect tissue reagent (ALL)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
+  </si>
+  <si>
+    <t>CLARITY hydrogel</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
+  </si>
+  <si>
+    <t>Neutral Buffered Formalin (NBF)</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBIB_0000213</t>
   </si>
   <si>
-    <t>Ethanol</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
-  </si>
-  <si>
-    <t>Allprotect tissue reagent (ALL)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000118</t>
-  </si>
-  <si>
-    <t>CLARITY hydrogel</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000134</t>
-  </si>
-  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -507,6 +513,15 @@
     <t>http://purl.obolibrary.org/obo/UO_0000082</t>
   </si>
   <si>
+    <t>is_rehydrated</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>notes</t>
   </si>
   <si>
@@ -531,7 +546,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-27T18:07:18-07:00</t>
+    <t>2023-12-13T11:46:15-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -590,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -613,6 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -626,7 +642,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -651,8 +667,9 @@
     <col min="17" max="17" style="18" width="21.1328125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" style="19" width="10.40625" customWidth="true" bestFit="true"/>
     <col min="19" max="19" style="20" width="9.25" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="5.94921875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="13.0703125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="5.94921875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -717,16 +734,19 @@
         <v>115</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="V1" t="s" s="1">
+        <v>119</v>
       </c>
     </row>
     <row r="2">
-      <c r="U2" t="s">
-        <v>117</v>
+      <c r="V2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
       <formula2/>
@@ -771,6 +791,9 @@
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'area_unit'!$A$1:$A$2</formula1>
     </dataValidation>
+    <dataValidation type="list" sqref="T2:T1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'is_rehydrated'!$A$1:$A$2</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
@@ -779,6 +802,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -794,30 +840,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1215,10 +1261,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Add new storage medium and preparation medium
Closes #46
</commit_message>
<xml_diff>
--- a/sample-section/latest/sample-section.xlsx
+++ b/sample-section/latest/sample-section.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
   <si>
     <t>source_id</t>
   </si>
@@ -279,6 +279,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000126</t>
   </si>
   <si>
+    <t>Alpha-MEM</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000371</t>
+  </si>
+  <si>
     <t>2% PFA/2.5% Glutaraldehyde</t>
   </si>
   <si>
@@ -315,6 +321,18 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
   </si>
   <si>
+    <t>Modified Davidson's Fixative</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000370</t>
+  </si>
+  <si>
+    <t>HPMC-PVP</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000386</t>
+  </si>
+  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -345,6 +363,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000198</t>
   </si>
   <si>
+    <t>Growth media</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000372</t>
+  </si>
+  <si>
     <t>RNAlater</t>
   </si>
   <si>
@@ -375,6 +399,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000147</t>
   </si>
   <si>
+    <t>Lysis buffer</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C178573</t>
+  </si>
+  <si>
     <t>preparation_condition</t>
   </si>
   <si>
@@ -435,6 +465,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
   </si>
   <si>
+    <t>Formic acid in water</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83719</t>
+  </si>
+  <si>
     <t>DMSO (no serum)</t>
   </si>
   <si>
@@ -480,6 +516,12 @@
     <t>storage_method</t>
   </si>
   <si>
+    <t>Stored in desiccator</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000387</t>
+  </si>
+  <si>
     <t>Incubated at 37 degrees celsius</t>
   </si>
   <si>
@@ -531,27 +573,27 @@
     <t>area_unit</t>
   </si>
   <si>
+    <t>mm^2</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000082</t>
+  </si>
+  <si>
     <t>um^2</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0010001</t>
   </si>
   <si>
-    <t>mm^2</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000082</t>
-  </si>
-  <si>
     <t>is_rehydrated</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -576,7 +618,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-18T09:38:41-07:00</t>
+    <t>2024-06-28T15:47:40-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -725,54 +767,54 @@
         <v>16</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -785,7 +827,7 @@
       <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$26</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$31</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -798,10 +840,10 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$20</formula1>
+      <formula1>'storage_medium'!$A$1:$A$22</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_method'!$A$1:$A$11</formula1>
+      <formula1>'storage_method'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -841,12 +883,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -870,30 +912,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +998,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1168,6 +1210,46 @@
       </c>
       <c r="B26" t="s" s="0">
         <v>68</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1185,34 +1267,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -1225,26 +1307,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1373,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1299,18 +1381,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
@@ -1323,10 +1405,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -1339,10 +1421,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -1355,106 +1437,122 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>30</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>96</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>66</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>38</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B21" t="s" s="0">
         <v>44</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1562,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1472,34 +1570,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -1512,50 +1610,58 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>79</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>66</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1573,26 +1679,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1610,18 +1716,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the "section index number" field's description
Closes #67
</commit_message>
<xml_diff>
--- a/sample-section/latest/sample-section.xlsx
+++ b/sample-section/latest/sample-section.xlsx
@@ -130,7 +130,8 @@
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The index number for the section if the sample is a single section.</t>
+        <t>(Required) The index number for the tissue section. The numbering of the tissue
+sections within a block should start with 1.</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
@@ -166,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="155">
   <si>
     <t>source_id</t>
   </si>
@@ -483,6 +484,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000135</t>
   </si>
   <si>
+    <t>Concentrated quench buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000391</t>
+  </si>
+  <si>
     <t>Gelatin</t>
   </si>
   <si>
@@ -618,7 +625,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-06-28T15:47:40-07:00</t>
+    <t>2025-01-23T09:53:47-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -779,42 +786,42 @@
         <v>96</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +847,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$22</formula1>
+      <formula1>'storage_medium'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="L2:L1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -883,12 +890,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -912,30 +919,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1380,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1469,18 +1476,18 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>34</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>106</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -1501,18 +1508,18 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>112</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -1525,33 +1532,41 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>74</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>40</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B23" t="s" s="0">
         <v>46</v>
       </c>
     </row>
@@ -1610,26 +1625,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9">
@@ -1679,26 +1694,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1716,18 +1731,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sample metadata templates
</commit_message>
<xml_diff>
--- a/sample-section/latest/sample-section.xlsx
+++ b/sample-section/latest/sample-section.xlsx
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="167">
   <si>
     <t>source_id</t>
   </si>
@@ -236,6 +236,12 @@
     <t>preparation_medium</t>
   </si>
   <si>
+    <t>HTK Solution</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000152</t>
+  </si>
+  <si>
     <t>NBF (Neutral Buffered Formalin)</t>
   </si>
   <si>
@@ -368,6 +374,12 @@
     <t>http://purl.bioontology.org/ontology/MESH/C046311</t>
   </si>
   <si>
+    <t>UW Solution</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000151</t>
+  </si>
+  <si>
     <t>MACS tissue storage solution</t>
   </si>
   <si>
@@ -473,6 +485,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000104</t>
   </si>
   <si>
+    <t>Stored on wet ice</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000465</t>
+  </si>
+  <si>
     <t>processing_time_value</t>
   </si>
   <si>
@@ -659,7 +677,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-16T07:27:11-07:00</t>
+    <t>2025-10-21T13:42:49-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -808,54 +826,54 @@
         <v>16</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
       <c r="V2" t="s" s="23">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -868,10 +886,10 @@
       <formula1>'source_storage_duration_unit'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$32</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_condition'!$A$1:$A$8</formula1>
+      <formula1>'preparation_condition'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -924,12 +942,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -953,30 +971,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1039,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1301,6 +1319,22 @@
         <v>80</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1308,7 +1342,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1316,66 +1350,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1430,202 +1472,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1643,98 +1685,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1752,26 +1794,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1789,18 +1831,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>